<commit_message>
guild & auction 完成 90 差测试
</commit_message>
<xml_diff>
--- a/src/main/resources/excel/monster/monster.xlsx
+++ b/src/main/resources/excel/monster/monster.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GitHub\MyFirstGame\src\main\resources\excel\monster\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8656A9A5-AD92-45C8-B2B2-AD95C567D8C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{73918EBE-3543-4D38-BFC2-144B40D46E67}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="7296" yWindow="1188" windowWidth="19008" windowHeight="10164" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2724" yWindow="984" windowWidth="19008" windowHeight="10164" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -75,10 +75,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>火焰哥布林</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>sensingRange</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -88,6 +84,10 @@
   </si>
   <si>
     <t>isAutoAttack</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>寒冰哥布林</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -416,7 +416,7 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -452,16 +452,16 @@
         <v>6</v>
       </c>
       <c r="I1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
         <v>13</v>
-      </c>
-      <c r="J1" t="s">
-        <v>14</v>
       </c>
       <c r="K1" t="s">
         <v>10</v>
       </c>
       <c r="L1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="M1" t="s">
         <v>11</v>
@@ -554,7 +554,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="C4">
         <v>10</v>

</xml_diff>